<commit_message>
Device changed to automation_device2
</commit_message>
<xml_diff>
--- a/Potman_Api/src/main/resources/API_Parameter.xlsx
+++ b/Potman_Api/src/main/resources/API_Parameter.xlsx
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2282" uniqueCount="236">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4482" uniqueCount="241">
   <si>
     <t xml:space="preserve">Request Packet </t>
   </si>
@@ -741,6 +741,21 @@
   </si>
   <si>
     <t>{"result":"Successful","collection_name":"Automation_Device2","data":[{"_id":"63e3294cf0f8f00771140c34","MP":{"EC":null,"MN_L":"Automation_Device2","MN":"Automation_Device2","MM":[0,1,2,3,4,5,6,7,8,9,10,11,12,13,14,15,16,17,18,19,20,21,22,23,24,25,26,27,28,29,30,31,32,33,34,35,36,37,38,39,40,41,42,43,44,45,46,47,48,49,50],"PQ":1,"DL":51,"PS":0,"PT":0,"CS":1,"SSS":0,"FI":1001,"MD":1,"MT":1},"NSS":1,"SD":0,"DT":"2023-02-08T10:17:08.000Z","UD":"","UI":"","GD":"1111","GI":"1111","MI":101,"name":[""],"meta":{"revision":0,"created":1675831628477,"version":0},"$loki":424}]}</t>
+  </si>
+  <si>
+    <t>{"key":"XaNoIaqF6okk3Kpf","request_type": "read_collection","collection_name": "MG2GFRP1_schedule_hour","limit": 1,"query": {}}</t>
+  </si>
+  <si>
+    <t>{"result":"Successful","collection_name":"MG2GFRP1_schedule_hour","data":[{"MI":22029810,"GI":"70B3D5253012","GD":"W-70B3D5253012","DT":"2023-02-08T12:47:58.000Z","SD":0,"NSS":93,"MP":{"MT":1,"MD":1,"FI":3130,"SSS":0,"CS":1,"PT":0,"PS":0,"DL":51,"PQ":4,"MN":"MG2GFRP1_schedule_hour","MN_L":"MG2GFRP1_schedule_hour","MM":[305,3626,"08:02:2023 11:47 AM - to: 08:02:2023 12:47 PM"],"EC":null},"others":{"opening_reading":[6725915,13021754],"closing_reading":[6726220,13025380]},"created_time":"2023-02-08T07:40:37.198Z","updated_time":"2023-02-08T07:40:37.198Z","name":["Energy (Wh)","Run Hours","CO2 (PPM)"],"meta":{"revision":0,"created":1675842037202,"version":0},"$loki":2424}]}</t>
+  </si>
+  <si>
+    <t>{"key":"OGQr1PegCcRcIWMq","request_type": "read_collection","collection_name": "MG2GFRP1_schedule_hour","limit": 1,"query": {}}</t>
+  </si>
+  <si>
+    <t>{"result":"Successful","collection_name":"MG2GFRP1_schedule_hour","data":[{"MI":22031218,"GI":"70B3D5253012","GD":"W-70B3D5253012","DT":"2023-02-08T15:47:15.000Z","SD":0,"NSS":93,"MP":{"MT":1,"MD":1,"FI":3130,"SSS":0,"CS":1,"PT":0,"PS":0,"DL":51,"PQ":4,"MN":"MG2GFRP1_schedule_hour","MN_L":"MG2GFRP1_schedule_hour","MM":[647,3600,"08:02:2023 2:47 PM - to: 08:02:2023 3:47 PM"],"EC":null},"others":{"opening_reading":[6728082,13032536],"closing_reading":[6728729,13036136]},"created_time":"2023-02-08T10:40:37.803Z","updated_time":"2023-02-08T10:40:37.803Z","name":["Energy (Wh)","Run Hours","CO2 (PPM)"],"meta":{"revision":0,"created":1675852837810,"version":0},"$loki":2427}]}</t>
+  </si>
+  <si>
+    <t>{"request_type":"read_collection","key":"OGQr1PegCcRcIWMq","message":"Maximum requests reached for the user!"}</t>
   </si>
 </sst>
 </file>
@@ -1117,11 +1132,11 @@
       <c r="B1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>1</v>
+      <c r="C1" t="s">
+        <v>238</v>
+      </c>
+      <c r="D1" t="s">
+        <v>240</v>
       </c>
       <c r="E1" s="1" t="s">
         <v>2</v>

</xml_diff>